<commit_message>
User Account Control window creation
</commit_message>
<xml_diff>
--- a/Library_Stock/Stock_Statement/Stock_inventory_template.xlsx
+++ b/Library_Stock/Stock_Statement/Stock_inventory_template.xlsx
@@ -684,7 +684,7 @@
       </c>
       <c r="D2" s="14" t="inlineStr">
         <is>
-          <t>Critical Stock</t>
+          <t>Commercial</t>
         </is>
       </c>
       <c r="G2" s="5" t="inlineStr">
@@ -694,7 +694,7 @@
       </c>
       <c r="H2" s="10" t="inlineStr">
         <is>
-          <t>20-May-2021</t>
+          <t>28-May-2021</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       <c r="B3" s="16" t="n"/>
       <c r="C3" s="8" t="inlineStr">
         <is>
-          <t>Rs.200</t>
+          <t>Rs.7018</t>
         </is>
       </c>
       <c r="G3" s="7" t="inlineStr">
@@ -717,7 +717,7 @@
       </c>
       <c r="H3" s="17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I3" s="16" t="n"/>

</xml_diff>

<commit_message>
Adding Item details print
</commit_message>
<xml_diff>
--- a/Library_Stock/Stock_Statement/Stock_inventory_template.xlsx
+++ b/Library_Stock/Stock_Statement/Stock_inventory_template.xlsx
@@ -694,7 +694,7 @@
       </c>
       <c r="H2" s="10" t="inlineStr">
         <is>
-          <t>28-May-2021</t>
+          <t>31-May-2021</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       <c r="B3" s="16" t="n"/>
       <c r="C3" s="8" t="inlineStr">
         <is>
-          <t>Rs.7018</t>
+          <t>Rs.7768</t>
         </is>
       </c>
       <c r="G3" s="7" t="inlineStr">

</xml_diff>